<commit_message>
Se agregan funcionalidades para el formulario de captura
</commit_message>
<xml_diff>
--- a/Dielmex Order Manager/Programacion-Excel.xlsx
+++ b/Dielmex Order Manager/Programacion-Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="7416" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17616" windowHeight="7416" tabRatio="638" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Precios" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="349">
   <si>
     <t>Descripción</t>
   </si>
@@ -1061,13 +1061,22 @@
     <t>Tecnico</t>
   </si>
   <si>
-    <t>ds</t>
-  </si>
-  <si>
     <t>jonh</t>
   </si>
   <si>
     <t>jenh</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>guadalajara</t>
+  </si>
+  <si>
+    <t>vallejon</t>
+  </si>
+  <si>
+    <t>jeny</t>
   </si>
 </sst>
 </file>
@@ -1667,60 +1676,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1731,6 +1686,60 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1754,59 +1763,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8.5"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1889,6 +1845,59 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8.5"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2582,27 +2591,10 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="132A89A151759014AEB184F216556CD900D221"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2265"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="15E57E5F1128D3144B71B706123362B4519C21"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19EA1E6DA1E9D1146951A77C16F0B7E97DAC71"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2610,6 +2602,23 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2096"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="974"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1487594CF1FC2C147F61B896146A81E4A150B1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3133"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2633,27 +2642,10 @@
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1487594CF1FC2C147F61B896146A81E4A150B1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3133"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19EA1E6DA1E9D1146951A77C16F0B7E97DAC71"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="15E57E5F1128D3144B71B706123362B4519C21"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2661,6 +2653,23 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2096"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="974"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="132A89A151759014AEB184F216556CD900D221"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2265"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2951,27 +2960,16 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
                     <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
-                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:tailEnd/>
                 </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -3135,26 +3133,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tbOrdenHeader" displayName="tbOrdenHeader" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tbOrdenHeader" displayName="tbOrdenHeader" ref="A1:G3" totalsRowShown="0">
+  <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No Orden"/>
-    <tableColumn id="11" name="No Equipo" dataDxfId="2"/>
+    <tableColumn id="11" name="No Equipo" dataDxfId="6"/>
     <tableColumn id="5" name="Centro de trabajo"/>
     <tableColumn id="6" name="Delegacion"/>
-    <tableColumn id="7" name="Fecha de Servicio" dataDxfId="1"/>
-    <tableColumn id="9" name="Tecnico" dataDxfId="6"/>
-    <tableColumn id="10" name="Recibio el servicio" dataDxfId="5"/>
+    <tableColumn id="7" name="Fecha de Servicio" dataDxfId="5"/>
+    <tableColumn id="9" name="Tecnico" dataDxfId="4"/>
+    <tableColumn id="10" name="Recibio el servicio" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tbOrdenBody" displayName="tbOrdenBody" ref="A1:E3" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tbOrdenBody" displayName="tbOrdenBody" ref="A1:E4" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Orden" dataDxfId="3"/>
+    <tableColumn id="1" name="Orden" dataDxfId="1"/>
     <tableColumn id="2" name="Clave" dataDxfId="0"/>
     <tableColumn id="3" name="Precio Unitario"/>
     <tableColumn id="4" name="Cantidad"/>
@@ -3430,8 +3428,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A3:F90"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5305,8 +5303,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6261,8 +6259,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6292,14 +6290,14 @@
       <c r="F3" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="D5" s="83" t="s">
+      <c r="B5" s="87"/>
+      <c r="D5" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="83"/>
+      <c r="E5" s="88"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -6314,10 +6312,10 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="89" t="s">
         <v>333</v>
       </c>
-      <c r="E7" s="84"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -6329,17 +6327,17 @@
         <v>1</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="84"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="100"/>
+      <c r="B10" s="82"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
     </row>
@@ -6348,10 +6346,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="83"/>
+      <c r="E11" s="88"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -6470,52 +6468,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="1039" r:id="rId4" name="_ActiveXWrapper21">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>891540</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>7620</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>15240</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>7620</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="1039" r:id="rId4" name="_ActiveXWrapper21"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="1034" r:id="rId6" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>190500</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>22860</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>15240</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>121920</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>167640</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>1150620</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>15240</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="1034" r:id="rId6" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6545,52 +6543,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId10" name="_ActiveXWrapper1">
+        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>22860</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>190500</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>1150620</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>121920</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>167640</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper21">
+        <control shapeId="1042" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>891540</xdr:colOff>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>7620</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>175260</xdr:rowOff>
+                <xdr:colOff>15240</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>7620</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper21"/>
+        <control shapeId="1042" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6613,30 +6611,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="43"/>
@@ -6668,17 +6666,17 @@
         <v>33</v>
       </c>
       <c r="B9" s="45"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
     </row>
     <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="95"/>
-      <c r="C10" s="95"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="93"/>
       <c r="D10" s="17" t="s">
         <v>35</v>
       </c>
@@ -6697,17 +6695,17 @@
       <c r="A12" s="22"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
@@ -6735,10 +6733,10 @@
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
       <c r="D17" s="29"/>
-      <c r="E17" s="96" t="s">
+      <c r="E17" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="96"/>
+      <c r="F17" s="94"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -6762,10 +6760,10 @@
         <v>42</v>
       </c>
       <c r="B21" s="13"/>
-      <c r="E21" s="87" t="s">
+      <c r="E21" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="87"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
@@ -6776,10 +6774,10 @@
       </c>
       <c r="B22" s="13"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="87" t="s">
+      <c r="E22" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="87"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -6788,41 +6786,41 @@
       <c r="A23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="89"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="90"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="97"/>
     </row>
     <row r="25" spans="1:9" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="88"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
-      <c r="H25" s="89"/>
-      <c r="I25" s="90"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="97"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="88" t="s">
+      <c r="A26" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="89"/>
-      <c r="H26" s="89"/>
-      <c r="I26" s="90"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="96"/>
+      <c r="I26" s="97"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="24"/>
@@ -6831,33 +6829,33 @@
       <c r="A28" s="25"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="86" t="s">
+      <c r="A29" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="94" t="s">
+      <c r="A31" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="94"/>
-      <c r="F31" s="94" t="s">
+      <c r="B31" s="92"/>
+      <c r="F31" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="91"/>
-      <c r="B32" s="91"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -6884,16 +6882,22 @@
       <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="86"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="100"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="85"/>
-      <c r="C38" s="86"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="100"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="17">
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="A31:B31"/>
@@ -6905,12 +6909,6 @@
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
@@ -6974,16 +6972,16 @@
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="104"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
@@ -7313,10 +7311,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7324,7 +7322,7 @@
     <col min="1" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="102" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="84" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="2.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.77734375" customWidth="1"/>
@@ -7344,7 +7342,7 @@
       <c r="D1" s="79" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="83" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="81" t="s">
@@ -7354,7 +7352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7365,18 +7363,41 @@
         <v>123</v>
       </c>
       <c r="D2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="83">
+        <v>42016</v>
+      </c>
+      <c r="F2" s="81" t="s">
         <v>343</v>
       </c>
-      <c r="E2" s="101">
-        <v>42016</v>
-      </c>
-      <c r="F2" s="81" t="s">
+      <c r="G2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>322</v>
+      </c>
+      <c r="C3">
+        <v>321</v>
+      </c>
+      <c r="D3" t="s">
         <v>345</v>
       </c>
-      <c r="H2" s="81"/>
+      <c r="E3" s="83">
+        <v>42351</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>347</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" s="81"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -7391,10 +7412,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja7"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7423,11 +7444,11 @@
       <c r="B2" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="103">
+      <c r="C2" s="86"/>
+      <c r="D2" s="85">
         <v>5</v>
       </c>
-      <c r="E2" s="103"/>
+      <c r="E2" s="85"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="81">
@@ -7438,6 +7459,18 @@
       </c>
       <c r="D3">
         <v>12</v>
+      </c>
+      <c r="E3" s="85"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="81">
+        <v>2</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya guarda en las tablas, hora de probar el primer prototipo
</commit_message>
<xml_diff>
--- a/Dielmex Order Manager/Programacion-Excel.xlsx
+++ b/Dielmex Order Manager/Programacion-Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16152" windowHeight="7416" tabRatio="638" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11016" windowHeight="7416" tabRatio="638" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Precios" sheetId="4" r:id="rId1"/>
@@ -1704,6 +1704,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1718,27 +1739,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2730,10 +2730,27 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="132A89A151759014AEB184F216556CD900D221"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2265"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19EA1E6DA1E9D1146951A77C16F0B7E97DAC71"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="15E57E5F1128D3144B71B706123362B4519C21"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2741,23 +2758,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2096"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="974"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1487594CF1FC2C147F61B896146A81E4A150B1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3133"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -2781,10 +2781,27 @@
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1487594CF1FC2C147F61B896146A81E4A150B1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3133"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="15E57E5F1128D3144B71B706123362B4519C21"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19EA1E6DA1E9D1146951A77C16F0B7E97DAC71"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -2792,23 +2809,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="2096"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="974"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="132A89A151759014AEB184F216556CD900D221"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2265"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="508"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -6416,7 +6416,7 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -6643,52 +6643,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId4" name="_ActiveXWrapper21">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>891540</xdr:colOff>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>7620</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>754380</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>175260</xdr:rowOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>15240</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>7620</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1039" r:id="rId4" name="_ActiveXWrapper21"/>
+        <control shapeId="1042" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId6" name="_ActiveXWrapper1">
+        <control shapeId="1041" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>22860</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>1150620</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>754380</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>167640</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId6" name="_ActiveXWrapper1"/>
+        <control shapeId="1041" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6718,52 +6718,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="1034" r:id="rId10" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>22860</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>15240</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>754380</xdr:colOff>
-                <xdr:row>15</xdr:row>
-                <xdr:rowOff>167640</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>1150620</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>15240</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="1034" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId12" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
+        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper21">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>891540</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>7620</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>15240</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>7620</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>754380</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1042" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper21"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6789,30 +6789,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="39"/>
@@ -6844,17 +6844,17 @@
         <v>33</v>
       </c>
       <c r="B9" s="41"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
     </row>
     <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="16" t="s">
         <v>35</v>
       </c>
@@ -6873,17 +6873,17 @@
       <c r="A12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
@@ -6911,10 +6911,10 @@
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="103" t="s">
+      <c r="E17" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="103"/>
+      <c r="F17" s="110"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
@@ -6938,10 +6938,10 @@
         <v>42</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="E21" s="107" t="s">
+      <c r="E21" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="107"/>
+      <c r="F21" s="101"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
@@ -6952,10 +6952,10 @@
       </c>
       <c r="B22" s="12"/>
       <c r="D22" s="28"/>
-      <c r="E22" s="107" t="s">
+      <c r="E22" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="107"/>
+      <c r="F22" s="101"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
@@ -6964,41 +6964,41 @@
       <c r="A23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="104" t="s">
+      <c r="A24" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="106"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="103"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="103"/>
+      <c r="H24" s="103"/>
+      <c r="I24" s="104"/>
     </row>
     <row r="25" spans="1:9" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="104"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="106"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="103"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="103"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="104"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="104" t="s">
+      <c r="A26" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="106"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="104"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
@@ -7007,33 +7007,33 @@
       <c r="A28" s="24"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="109"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="109"/>
-      <c r="G29" s="109"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
     </row>
     <row r="31" spans="1:9" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="101"/>
-      <c r="F31" s="101" t="s">
+      <c r="B31" s="108"/>
+      <c r="F31" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="108"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="110"/>
-      <c r="B32" s="110"/>
+      <c r="A32" s="105"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -7060,22 +7060,16 @@
       <c r="A37" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="108"/>
-      <c r="C37" s="109"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="100"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="108"/>
-      <c r="C38" s="109"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="100"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="17">
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="A31:B31"/>
@@ -7087,6 +7081,12 @@
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
@@ -7491,7 +7491,7 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -7552,7 +7552,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>